<commit_message>
Added Diagrammes d'occurences et cardinalités
</commit_message>
<xml_diff>
--- a/Gestion du temps.xlsx
+++ b/Gestion du temps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>demi-journée</t>
   </si>
@@ -143,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -166,11 +166,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -182,6 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,7 +685,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>26</v>
@@ -683,7 +695,7 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>-12</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -749,6 +761,22 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Folder cleanup before last commit
</commit_message>
<xml_diff>
--- a/Gestion du temps.xlsx
+++ b/Gestion du temps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>demi-journée</t>
   </si>
@@ -156,13 +156,16 @@
   </si>
   <si>
     <t>sans objet</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +182,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -239,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -270,6 +283,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,7 +573,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G15" si="0">D3-F3</f>
+        <f t="shared" ref="G3:G13" si="0">D3-F3</f>
         <v>6</v>
       </c>
     </row>
@@ -886,11 +905,22 @@
       <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="C14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="11">
+        <f>SUM(D2:D13)</f>
+        <v>97</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11">
+        <f>SUM(F2:F13)</f>
+        <v>81</v>
+      </c>
+      <c r="G14" s="11">
+        <f>SUM(G2:G13)</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">

</xml_diff>

<commit_message>
Added & finished Powerpoint
</commit_message>
<xml_diff>
--- a/Gestion du temps.xlsx
+++ b/Gestion du temps.xlsx
@@ -77,9 +77,6 @@
     <t>Prise de connaissance</t>
   </si>
   <si>
-    <t>temps estimé par tâche en heures</t>
-  </si>
-  <si>
     <t>use case</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>temps passé</t>
   </si>
 </sst>
 </file>
@@ -570,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,7 +587,7 @@
     <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -595,22 +595,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -624,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3">
         <v>4</v>
@@ -634,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -642,13 +642,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="3">
         <v>4</v>
@@ -657,8 +657,12 @@
         <f t="shared" ref="G3:G13" si="0">D3-F3</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <f>11+8+25+12+21+12</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -666,13 +670,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3">
         <v>16</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3">
         <v>10</v>
@@ -682,7 +686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -690,13 +694,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3">
         <v>3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3">
         <v>4</v>
@@ -706,7 +710,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -714,13 +718,13 @@
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3">
         <v>0.5</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -730,7 +734,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -738,13 +742,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3">
         <v>16</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3">
         <v>10</v>
@@ -754,7 +758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -762,13 +766,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3">
         <v>8</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3">
         <v>10</v>
@@ -778,7 +782,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -786,13 +790,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3">
         <v>22</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3">
         <v>20</v>
@@ -802,7 +806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -810,13 +814,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3">
         <v>0.5</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3">
         <v>2</v>
@@ -826,7 +830,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -834,13 +838,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3">
         <v>12</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="3">
         <v>10</v>
@@ -850,7 +854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -858,13 +862,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="8">
         <v>2</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="8">
         <v>2</v>
@@ -874,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -882,13 +886,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="8">
         <v>3</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="8">
         <v>4</v>
@@ -898,7 +902,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -906,7 +910,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="11">
         <f>SUM(D2:D13)</f>
@@ -922,7 +926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -935,7 +939,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -966,7 +970,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -979,7 +983,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -992,7 +996,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1005,7 +1009,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1018,7 +1022,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1031,7 +1035,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -1044,7 +1048,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>

</xml_diff>